<commit_message>
ubah prompt engineering menjadi zero-shot
</commit_message>
<xml_diff>
--- a/data/responses.xlsx
+++ b/data/responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AV48"/>
+  <dimension ref="A1:AV49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6769,10 +6769,8 @@
           <t>2025-05-16 14:53:10</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>34</t>
-        </is>
+      <c r="B48" t="n">
+        <v>34</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -6794,214 +6792,372 @@
           <t>bism</t>
         </is>
       </c>
-      <c r="G48" t="inlineStr">
+      <c r="G48" t="n">
+        <v>2</v>
+      </c>
+      <c r="H48" t="n">
+        <v>3</v>
+      </c>
+      <c r="I48" t="n">
+        <v>2</v>
+      </c>
+      <c r="J48" t="n">
+        <v>3</v>
+      </c>
+      <c r="K48" t="n">
+        <v>2</v>
+      </c>
+      <c r="L48" t="n">
+        <v>2</v>
+      </c>
+      <c r="M48" t="n">
+        <v>1</v>
+      </c>
+      <c r="N48" t="n">
+        <v>2</v>
+      </c>
+      <c r="O48" t="n">
+        <v>2</v>
+      </c>
+      <c r="P48" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q48" t="n">
+        <v>2</v>
+      </c>
+      <c r="R48" t="n">
+        <v>2</v>
+      </c>
+      <c r="S48" t="n">
+        <v>1</v>
+      </c>
+      <c r="T48" t="n">
+        <v>2</v>
+      </c>
+      <c r="U48" t="n">
+        <v>2</v>
+      </c>
+      <c r="V48" t="n">
+        <v>3</v>
+      </c>
+      <c r="W48" t="n">
+        <v>2</v>
+      </c>
+      <c r="X48" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y48" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z48" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB48" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC48" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD48" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF48" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG48" t="n">
+        <v>3</v>
+      </c>
+      <c r="AH48" t="n">
+        <v>2</v>
+      </c>
+      <c r="AI48" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ48" t="n">
+        <v>3</v>
+      </c>
+      <c r="AK48" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM48" t="n">
+        <v>2</v>
+      </c>
+      <c r="AN48" t="n">
+        <v>3</v>
+      </c>
+      <c r="AO48" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP48" t="n">
+        <v>2</v>
+      </c>
+      <c r="AQ48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR48" t="n">
+        <v>2</v>
+      </c>
+      <c r="AS48" t="n">
+        <v>2</v>
+      </c>
+      <c r="AT48" t="n">
+        <v>2</v>
+      </c>
+      <c r="AU48" t="n">
+        <v>3</v>
+      </c>
+      <c r="AV48" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2025-05-16 14:59:19</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Bali, Indonesia</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>D3</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>dsada</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="H48" t="inlineStr">
+      <c r="K49" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="I48" t="inlineStr">
+      <c r="L49" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="J48" t="inlineStr">
+      <c r="M49" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="K48" t="inlineStr">
+      <c r="N49" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="L48" t="inlineStr">
+      <c r="O49" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="M48" t="inlineStr">
+      <c r="P49" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Q49" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="R49" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="S49" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="T49" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="N48" t="inlineStr">
+      <c r="U49" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="O48" t="inlineStr">
+      <c r="V49" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="W49" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="P48" t="inlineStr">
+      <c r="X49" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="Q48" t="inlineStr">
+      <c r="Y49" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="R48" t="inlineStr">
+      <c r="Z49" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="S48" t="inlineStr">
+      <c r="AA49" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AB49" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="AC49" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="T48" t="inlineStr">
+      <c r="AD49" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="U48" t="inlineStr">
+      <c r="AE49" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="AF49" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="V48" t="inlineStr">
+      <c r="AG49" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AH49" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AI49" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="W48" t="inlineStr">
+      <c r="AJ49" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="X48" t="inlineStr">
+      <c r="AK49" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AL49" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="Y48" t="inlineStr">
+      <c r="AM49" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AN49" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="Z48" t="inlineStr">
+      <c r="AO49" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="AA48" t="inlineStr">
+      <c r="AP49" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AQ49" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="AB48" t="inlineStr">
+      <c r="AR49" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="AC48" t="inlineStr">
+      <c r="AS49" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AT49" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="AD48" t="inlineStr">
+      <c r="AU49" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="AE48" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AF48" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AG48" t="inlineStr">
+      <c r="AV49" t="inlineStr">
         <is>
           <t>3</t>
-        </is>
-      </c>
-      <c r="AH48" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AI48" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AJ48" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="AK48" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AL48" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AM48" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AN48" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="AO48" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AP48" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AQ48" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AR48" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AS48" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AT48" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AU48" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="AV48" t="inlineStr">
-        <is>
-          <t>2</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
pembaruan format interpretasi hasil
</commit_message>
<xml_diff>
--- a/data/responses.xlsx
+++ b/data/responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AV51"/>
+  <dimension ref="A1:AV52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7237,237 +7237,393 @@
           <t>2025-05-21 10:00:03</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr">
+      <c r="B51" t="n">
+        <v>34</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Medan</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>SMA/SMK</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Dragahalo</t>
+        </is>
+      </c>
+      <c r="G51" t="n">
+        <v>3</v>
+      </c>
+      <c r="H51" t="n">
+        <v>2</v>
+      </c>
+      <c r="I51" t="n">
+        <v>3</v>
+      </c>
+      <c r="J51" t="n">
+        <v>2</v>
+      </c>
+      <c r="K51" t="n">
+        <v>3</v>
+      </c>
+      <c r="L51" t="n">
+        <v>2</v>
+      </c>
+      <c r="M51" t="n">
+        <v>2</v>
+      </c>
+      <c r="N51" t="n">
+        <v>1</v>
+      </c>
+      <c r="O51" t="n">
+        <v>2</v>
+      </c>
+      <c r="P51" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q51" t="n">
+        <v>1</v>
+      </c>
+      <c r="R51" t="n">
+        <v>2</v>
+      </c>
+      <c r="S51" t="n">
+        <v>1</v>
+      </c>
+      <c r="T51" t="n">
+        <v>2</v>
+      </c>
+      <c r="U51" t="n">
+        <v>1</v>
+      </c>
+      <c r="V51" t="n">
+        <v>2</v>
+      </c>
+      <c r="W51" t="n">
+        <v>3</v>
+      </c>
+      <c r="X51" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y51" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z51" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA51" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB51" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC51" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD51" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE51" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF51" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG51" t="n">
+        <v>2</v>
+      </c>
+      <c r="AH51" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI51" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ51" t="n">
+        <v>2</v>
+      </c>
+      <c r="AK51" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL51" t="n">
+        <v>2</v>
+      </c>
+      <c r="AM51" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN51" t="n">
+        <v>2</v>
+      </c>
+      <c r="AO51" t="n">
+        <v>3</v>
+      </c>
+      <c r="AP51" t="n">
+        <v>2</v>
+      </c>
+      <c r="AQ51" t="n">
+        <v>2</v>
+      </c>
+      <c r="AR51" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS51" t="n">
+        <v>2</v>
+      </c>
+      <c r="AT51" t="n">
+        <v>2</v>
+      </c>
+      <c r="AU51" t="n">
+        <v>3</v>
+      </c>
+      <c r="AV51" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2025-05-21 10:34:00</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
         <is>
           <t>34</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>Medan</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Jakarta</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
         <is>
           <t>SMA/SMK</t>
         </is>
       </c>
-      <c r="E51" t="inlineStr">
+      <c r="E52" t="inlineStr">
         <is>
           <t>male</t>
         </is>
       </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>Dragahalo</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>dasdsd</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="H51" t="inlineStr">
+      <c r="I52" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="I51" t="inlineStr">
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="J51" t="inlineStr">
+      <c r="L52" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="K51" t="inlineStr">
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="N52" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="P52" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Q52" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="L51" t="inlineStr">
+      <c r="R52" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="M51" t="inlineStr">
+      <c r="S52" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="N51" t="inlineStr">
+      <c r="T52" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="U52" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="V52" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="O51" t="inlineStr">
+      <c r="W52" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="P51" t="inlineStr">
+      <c r="X52" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="Y52" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="Q51" t="inlineStr">
+      <c r="Z52" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="AA52" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AB52" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AC52" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="AD52" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AE52" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="R51" t="inlineStr">
+      <c r="AF52" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="S51" t="inlineStr">
+      <c r="AG52" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="AH52" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AI52" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AJ52" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AK52" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="AL52" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AM52" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AN52" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AO52" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="T51" t="inlineStr">
+      <c r="AP52" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="U51" t="inlineStr">
+      <c r="AQ52" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AR52" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="AS52" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AT52" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="V51" t="inlineStr">
+      <c r="AU52" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="W51" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="X51" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="Y51" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="Z51" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AA51" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AB51" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="AC51" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AD51" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AE51" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AF51" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AG51" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AH51" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AI51" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AJ51" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AK51" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AL51" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AM51" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AN51" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AO51" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="AP51" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AQ51" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AR51" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AS51" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AT51" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AU51" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="AV51" t="inlineStr">
+      <c r="AV52" t="inlineStr">
         <is>
           <t>2</t>
         </is>

</xml_diff>

<commit_message>
sertifikat hanya skor diintegrasikan dengan chatbot
</commit_message>
<xml_diff>
--- a/data/responses.xlsx
+++ b/data/responses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AV52"/>
+  <dimension ref="A1:AV59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7393,10 +7393,8 @@
           <t>2025-05-21 10:34:00</t>
         </is>
       </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>34</t>
-        </is>
+      <c r="B52" t="n">
+        <v>34</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -7418,212 +7416,1306 @@
           <t>dasdsd</t>
         </is>
       </c>
-      <c r="G52" t="inlineStr">
+      <c r="G52" t="n">
+        <v>2</v>
+      </c>
+      <c r="H52" t="n">
+        <v>3</v>
+      </c>
+      <c r="I52" t="n">
+        <v>2</v>
+      </c>
+      <c r="J52" t="n">
+        <v>2</v>
+      </c>
+      <c r="K52" t="n">
+        <v>3</v>
+      </c>
+      <c r="L52" t="n">
+        <v>2</v>
+      </c>
+      <c r="M52" t="n">
+        <v>2</v>
+      </c>
+      <c r="N52" t="n">
+        <v>2</v>
+      </c>
+      <c r="O52" t="n">
+        <v>1</v>
+      </c>
+      <c r="P52" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q52" t="n">
+        <v>3</v>
+      </c>
+      <c r="R52" t="n">
+        <v>2</v>
+      </c>
+      <c r="S52" t="n">
+        <v>2</v>
+      </c>
+      <c r="T52" t="n">
+        <v>3</v>
+      </c>
+      <c r="U52" t="n">
+        <v>2</v>
+      </c>
+      <c r="V52" t="n">
+        <v>1</v>
+      </c>
+      <c r="W52" t="n">
+        <v>2</v>
+      </c>
+      <c r="X52" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y52" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z52" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA52" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB52" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC52" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD52" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE52" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF52" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG52" t="n">
+        <v>3</v>
+      </c>
+      <c r="AH52" t="n">
+        <v>2</v>
+      </c>
+      <c r="AI52" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ52" t="n">
+        <v>2</v>
+      </c>
+      <c r="AK52" t="n">
+        <v>3</v>
+      </c>
+      <c r="AL52" t="n">
+        <v>2</v>
+      </c>
+      <c r="AM52" t="n">
+        <v>2</v>
+      </c>
+      <c r="AN52" t="n">
+        <v>2</v>
+      </c>
+      <c r="AO52" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP52" t="n">
+        <v>2</v>
+      </c>
+      <c r="AQ52" t="n">
+        <v>2</v>
+      </c>
+      <c r="AR52" t="n">
+        <v>3</v>
+      </c>
+      <c r="AS52" t="n">
+        <v>2</v>
+      </c>
+      <c r="AT52" t="n">
+        <v>1</v>
+      </c>
+      <c r="AU52" t="n">
+        <v>2</v>
+      </c>
+      <c r="AV52" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2025-05-24 22:59:53</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>34</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Bali, Indonesia</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>SMA/SMK</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>jimmnnkk</t>
+        </is>
+      </c>
+      <c r="G53" t="n">
+        <v>3</v>
+      </c>
+      <c r="H53" t="n">
+        <v>2</v>
+      </c>
+      <c r="I53" t="n">
+        <v>3</v>
+      </c>
+      <c r="J53" t="n">
+        <v>2</v>
+      </c>
+      <c r="K53" t="n">
+        <v>2</v>
+      </c>
+      <c r="L53" t="n">
+        <v>3</v>
+      </c>
+      <c r="M53" t="n">
+        <v>2</v>
+      </c>
+      <c r="N53" t="n">
+        <v>3</v>
+      </c>
+      <c r="O53" t="n">
+        <v>2</v>
+      </c>
+      <c r="P53" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q53" t="n">
+        <v>1</v>
+      </c>
+      <c r="R53" t="n">
+        <v>2</v>
+      </c>
+      <c r="S53" t="n">
+        <v>2</v>
+      </c>
+      <c r="T53" t="n">
+        <v>1</v>
+      </c>
+      <c r="U53" t="n">
+        <v>2</v>
+      </c>
+      <c r="V53" t="n">
+        <v>2</v>
+      </c>
+      <c r="W53" t="n">
+        <v>1</v>
+      </c>
+      <c r="X53" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y53" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z53" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA53" t="n">
+        <v>2</v>
+      </c>
+      <c r="AB53" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC53" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD53" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE53" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF53" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG53" t="n">
+        <v>2</v>
+      </c>
+      <c r="AH53" t="n">
+        <v>3</v>
+      </c>
+      <c r="AI53" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ53" t="n">
+        <v>2</v>
+      </c>
+      <c r="AK53" t="n">
+        <v>3</v>
+      </c>
+      <c r="AL53" t="n">
+        <v>2</v>
+      </c>
+      <c r="AM53" t="n">
+        <v>2</v>
+      </c>
+      <c r="AN53" t="n">
+        <v>3</v>
+      </c>
+      <c r="AO53" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP53" t="n">
+        <v>2</v>
+      </c>
+      <c r="AQ53" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR53" t="n">
+        <v>2</v>
+      </c>
+      <c r="AS53" t="n">
+        <v>3</v>
+      </c>
+      <c r="AT53" t="n">
+        <v>2</v>
+      </c>
+      <c r="AU53" t="n">
+        <v>2</v>
+      </c>
+      <c r="AV53" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2025-05-26 11:37:50</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>45</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Jakarta</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>SMA/SMK</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>M. Rakhmat Dramaga</t>
+        </is>
+      </c>
+      <c r="G54" t="n">
+        <v>2</v>
+      </c>
+      <c r="H54" t="n">
+        <v>3</v>
+      </c>
+      <c r="I54" t="n">
+        <v>2</v>
+      </c>
+      <c r="J54" t="n">
+        <v>3</v>
+      </c>
+      <c r="K54" t="n">
+        <v>2</v>
+      </c>
+      <c r="L54" t="n">
+        <v>3</v>
+      </c>
+      <c r="M54" t="n">
+        <v>3</v>
+      </c>
+      <c r="N54" t="n">
+        <v>3</v>
+      </c>
+      <c r="O54" t="n">
+        <v>3</v>
+      </c>
+      <c r="P54" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q54" t="n">
+        <v>3</v>
+      </c>
+      <c r="R54" t="n">
+        <v>2</v>
+      </c>
+      <c r="S54" t="n">
+        <v>4</v>
+      </c>
+      <c r="T54" t="n">
+        <v>3</v>
+      </c>
+      <c r="U54" t="n">
+        <v>3</v>
+      </c>
+      <c r="V54" t="n">
+        <v>2</v>
+      </c>
+      <c r="W54" t="n">
+        <v>3</v>
+      </c>
+      <c r="X54" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y54" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z54" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA54" t="n">
+        <v>4</v>
+      </c>
+      <c r="AB54" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC54" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD54" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE54" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF54" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG54" t="n">
+        <v>3</v>
+      </c>
+      <c r="AH54" t="n">
+        <v>2</v>
+      </c>
+      <c r="AI54" t="n">
+        <v>3</v>
+      </c>
+      <c r="AJ54" t="n">
+        <v>4</v>
+      </c>
+      <c r="AK54" t="n">
+        <v>3</v>
+      </c>
+      <c r="AL54" t="n">
+        <v>2</v>
+      </c>
+      <c r="AM54" t="n">
+        <v>3</v>
+      </c>
+      <c r="AN54" t="n">
+        <v>2</v>
+      </c>
+      <c r="AO54" t="n">
+        <v>3</v>
+      </c>
+      <c r="AP54" t="n">
+        <v>3</v>
+      </c>
+      <c r="AQ54" t="n">
+        <v>2</v>
+      </c>
+      <c r="AR54" t="n">
+        <v>3</v>
+      </c>
+      <c r="AS54" t="n">
+        <v>3</v>
+      </c>
+      <c r="AT54" t="n">
+        <v>2</v>
+      </c>
+      <c r="AU54" t="n">
+        <v>2</v>
+      </c>
+      <c r="AV54" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2025-05-26 11:48:38</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>45</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Jakarta</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>SMA/SMK</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>M. Rakhmat Dramaga</t>
+        </is>
+      </c>
+      <c r="G55" t="n">
+        <v>4</v>
+      </c>
+      <c r="H55" t="n">
+        <v>4</v>
+      </c>
+      <c r="I55" t="n">
+        <v>4</v>
+      </c>
+      <c r="J55" t="n">
+        <v>4</v>
+      </c>
+      <c r="K55" t="n">
+        <v>4</v>
+      </c>
+      <c r="L55" t="n">
+        <v>4</v>
+      </c>
+      <c r="M55" t="n">
+        <v>4</v>
+      </c>
+      <c r="N55" t="n">
+        <v>4</v>
+      </c>
+      <c r="O55" t="n">
+        <v>4</v>
+      </c>
+      <c r="P55" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q55" t="n">
+        <v>4</v>
+      </c>
+      <c r="R55" t="n">
+        <v>4</v>
+      </c>
+      <c r="S55" t="n">
+        <v>4</v>
+      </c>
+      <c r="T55" t="n">
+        <v>4</v>
+      </c>
+      <c r="U55" t="n">
+        <v>4</v>
+      </c>
+      <c r="V55" t="n">
+        <v>4</v>
+      </c>
+      <c r="W55" t="n">
+        <v>4</v>
+      </c>
+      <c r="X55" t="n">
+        <v>4</v>
+      </c>
+      <c r="Y55" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z55" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA55" t="n">
+        <v>4</v>
+      </c>
+      <c r="AB55" t="n">
+        <v>4</v>
+      </c>
+      <c r="AC55" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD55" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE55" t="n">
+        <v>4</v>
+      </c>
+      <c r="AF55" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG55" t="n">
+        <v>4</v>
+      </c>
+      <c r="AH55" t="n">
+        <v>4</v>
+      </c>
+      <c r="AI55" t="n">
+        <v>4</v>
+      </c>
+      <c r="AJ55" t="n">
+        <v>4</v>
+      </c>
+      <c r="AK55" t="n">
+        <v>4</v>
+      </c>
+      <c r="AL55" t="n">
+        <v>4</v>
+      </c>
+      <c r="AM55" t="n">
+        <v>4</v>
+      </c>
+      <c r="AN55" t="n">
+        <v>4</v>
+      </c>
+      <c r="AO55" t="n">
+        <v>4</v>
+      </c>
+      <c r="AP55" t="n">
+        <v>4</v>
+      </c>
+      <c r="AQ55" t="n">
+        <v>4</v>
+      </c>
+      <c r="AR55" t="n">
+        <v>4</v>
+      </c>
+      <c r="AS55" t="n">
+        <v>4</v>
+      </c>
+      <c r="AT55" t="n">
+        <v>4</v>
+      </c>
+      <c r="AU55" t="n">
+        <v>4</v>
+      </c>
+      <c r="AV55" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2025-05-26 11:57:52</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>23</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Medan</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>SMA/SMK</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Bahteramon</t>
+        </is>
+      </c>
+      <c r="G56" t="n">
+        <v>2</v>
+      </c>
+      <c r="H56" t="n">
+        <v>3</v>
+      </c>
+      <c r="I56" t="n">
+        <v>3</v>
+      </c>
+      <c r="J56" t="n">
+        <v>2</v>
+      </c>
+      <c r="K56" t="n">
+        <v>3</v>
+      </c>
+      <c r="L56" t="n">
+        <v>2</v>
+      </c>
+      <c r="M56" t="n">
+        <v>3</v>
+      </c>
+      <c r="N56" t="n">
+        <v>3</v>
+      </c>
+      <c r="O56" t="n">
+        <v>2</v>
+      </c>
+      <c r="P56" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q56" t="n">
+        <v>3</v>
+      </c>
+      <c r="R56" t="n">
+        <v>2</v>
+      </c>
+      <c r="S56" t="n">
+        <v>3</v>
+      </c>
+      <c r="T56" t="n">
+        <v>4</v>
+      </c>
+      <c r="U56" t="n">
+        <v>3</v>
+      </c>
+      <c r="V56" t="n">
+        <v>4</v>
+      </c>
+      <c r="W56" t="n">
+        <v>3</v>
+      </c>
+      <c r="X56" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y56" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z56" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA56" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB56" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC56" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD56" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE56" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF56" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG56" t="n">
+        <v>3</v>
+      </c>
+      <c r="AH56" t="n">
+        <v>4</v>
+      </c>
+      <c r="AI56" t="n">
+        <v>3</v>
+      </c>
+      <c r="AJ56" t="n">
+        <v>3</v>
+      </c>
+      <c r="AK56" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL56" t="n">
+        <v>3</v>
+      </c>
+      <c r="AM56" t="n">
+        <v>3</v>
+      </c>
+      <c r="AN56" t="n">
+        <v>4</v>
+      </c>
+      <c r="AO56" t="n">
+        <v>3</v>
+      </c>
+      <c r="AP56" t="n">
+        <v>2</v>
+      </c>
+      <c r="AQ56" t="n">
+        <v>3</v>
+      </c>
+      <c r="AR56" t="n">
+        <v>4</v>
+      </c>
+      <c r="AS56" t="n">
+        <v>3</v>
+      </c>
+      <c r="AT56" t="n">
+        <v>2</v>
+      </c>
+      <c r="AU56" t="n">
+        <v>3</v>
+      </c>
+      <c r="AV56" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2025-05-26 15:01:19</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>23</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Medan</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>SMA/SMK</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Bahteramon</t>
+        </is>
+      </c>
+      <c r="G57" t="n">
+        <v>3</v>
+      </c>
+      <c r="H57" t="n">
+        <v>3</v>
+      </c>
+      <c r="I57" t="n">
+        <v>3</v>
+      </c>
+      <c r="J57" t="n">
+        <v>2</v>
+      </c>
+      <c r="K57" t="n">
+        <v>3</v>
+      </c>
+      <c r="L57" t="n">
+        <v>3</v>
+      </c>
+      <c r="M57" t="n">
+        <v>3</v>
+      </c>
+      <c r="N57" t="n">
+        <v>2</v>
+      </c>
+      <c r="O57" t="n">
+        <v>3</v>
+      </c>
+      <c r="P57" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q57" t="n">
+        <v>3</v>
+      </c>
+      <c r="R57" t="n">
+        <v>3</v>
+      </c>
+      <c r="S57" t="n">
+        <v>3</v>
+      </c>
+      <c r="T57" t="n">
+        <v>3</v>
+      </c>
+      <c r="U57" t="n">
+        <v>3</v>
+      </c>
+      <c r="V57" t="n">
+        <v>2</v>
+      </c>
+      <c r="W57" t="n">
+        <v>3</v>
+      </c>
+      <c r="X57" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y57" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z57" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA57" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB57" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC57" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD57" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE57" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF57" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG57" t="n">
+        <v>3</v>
+      </c>
+      <c r="AH57" t="n">
+        <v>2</v>
+      </c>
+      <c r="AI57" t="n">
+        <v>3</v>
+      </c>
+      <c r="AJ57" t="n">
+        <v>2</v>
+      </c>
+      <c r="AK57" t="n">
+        <v>3</v>
+      </c>
+      <c r="AL57" t="n">
+        <v>2</v>
+      </c>
+      <c r="AM57" t="n">
+        <v>3</v>
+      </c>
+      <c r="AN57" t="n">
+        <v>3</v>
+      </c>
+      <c r="AO57" t="n">
+        <v>3</v>
+      </c>
+      <c r="AP57" t="n">
+        <v>3</v>
+      </c>
+      <c r="AQ57" t="n">
+        <v>4</v>
+      </c>
+      <c r="AR57" t="n">
+        <v>3</v>
+      </c>
+      <c r="AS57" t="n">
+        <v>2</v>
+      </c>
+      <c r="AT57" t="n">
+        <v>3</v>
+      </c>
+      <c r="AU57" t="n">
+        <v>2</v>
+      </c>
+      <c r="AV57" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2025-05-26 15:12:41</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>23</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Medan</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>SMA/SMK</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Bahteramon</t>
+        </is>
+      </c>
+      <c r="G58" t="n">
+        <v>3</v>
+      </c>
+      <c r="H58" t="n">
+        <v>3</v>
+      </c>
+      <c r="I58" t="n">
+        <v>2</v>
+      </c>
+      <c r="J58" t="n">
+        <v>3</v>
+      </c>
+      <c r="K58" t="n">
+        <v>3</v>
+      </c>
+      <c r="L58" t="n">
+        <v>2</v>
+      </c>
+      <c r="M58" t="n">
+        <v>3</v>
+      </c>
+      <c r="N58" t="n">
+        <v>2</v>
+      </c>
+      <c r="O58" t="n">
+        <v>3</v>
+      </c>
+      <c r="P58" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q58" t="n">
+        <v>3</v>
+      </c>
+      <c r="R58" t="n">
+        <v>4</v>
+      </c>
+      <c r="S58" t="n">
+        <v>3</v>
+      </c>
+      <c r="T58" t="n">
+        <v>2</v>
+      </c>
+      <c r="U58" t="n">
+        <v>3</v>
+      </c>
+      <c r="V58" t="n">
+        <v>2</v>
+      </c>
+      <c r="W58" t="n">
+        <v>3</v>
+      </c>
+      <c r="X58" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y58" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z58" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA58" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB58" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC58" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD58" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE58" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF58" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG58" t="n">
+        <v>3</v>
+      </c>
+      <c r="AH58" t="n">
+        <v>2</v>
+      </c>
+      <c r="AI58" t="n">
+        <v>3</v>
+      </c>
+      <c r="AJ58" t="n">
+        <v>4</v>
+      </c>
+      <c r="AK58" t="n">
+        <v>3</v>
+      </c>
+      <c r="AL58" t="n">
+        <v>2</v>
+      </c>
+      <c r="AM58" t="n">
+        <v>3</v>
+      </c>
+      <c r="AN58" t="n">
+        <v>2</v>
+      </c>
+      <c r="AO58" t="n">
+        <v>3</v>
+      </c>
+      <c r="AP58" t="n">
+        <v>2</v>
+      </c>
+      <c r="AQ58" t="n">
+        <v>3</v>
+      </c>
+      <c r="AR58" t="n">
+        <v>2</v>
+      </c>
+      <c r="AS58" t="n">
+        <v>3</v>
+      </c>
+      <c r="AT58" t="n">
+        <v>2</v>
+      </c>
+      <c r="AU58" t="n">
+        <v>3</v>
+      </c>
+      <c r="AV58" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2025-05-26 15:20:11</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Medan</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>SMP</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Bahteramon</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="M59" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="H52" t="inlineStr">
+      <c r="N59" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="I52" t="inlineStr">
+      <c r="O59" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="J52" t="inlineStr">
+      <c r="P59" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="Q59" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="R59" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="S59" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="K52" t="inlineStr">
+      <c r="T59" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="L52" t="inlineStr">
+      <c r="U59" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="V59" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="M52" t="inlineStr">
+      <c r="W59" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="X59" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="N52" t="inlineStr">
+      <c r="Y59" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="Z59" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="O52" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="P52" t="inlineStr">
+      <c r="AA59" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="AB59" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="Q52" t="inlineStr">
+      <c r="AC59" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="R52" t="inlineStr">
+      <c r="AD59" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="S52" t="inlineStr">
+      <c r="AE59" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="AF59" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="T52" t="inlineStr">
+      <c r="AG59" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="U52" t="inlineStr">
+      <c r="AH59" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="V52" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="W52" t="inlineStr">
+      <c r="AI59" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="AJ59" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="X52" t="inlineStr">
+      <c r="AK59" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="Y52" t="inlineStr">
+      <c r="AL59" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="Z52" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="AA52" t="inlineStr">
+      <c r="AM59" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="AB52" t="inlineStr">
+      <c r="AN59" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="AC52" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="AD52" t="inlineStr">
+      <c r="AO59" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="AE52" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AF52" t="inlineStr">
+      <c r="AP59" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="AG52" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="AH52" t="inlineStr">
+      <c r="AQ59" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="AI52" t="inlineStr">
+      <c r="AR59" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="AJ52" t="inlineStr">
+      <c r="AS59" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="AK52" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="AL52" t="inlineStr">
+      <c r="AT59" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="AM52" t="inlineStr">
+      <c r="AU59" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="AN52" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AO52" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AP52" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AQ52" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AR52" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="AS52" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AT52" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AU52" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AV52" t="inlineStr">
+      <c r="AV59" t="inlineStr">
         <is>
           <t>2</t>
         </is>

</xml_diff>